<commit_message>
data till 22 Feb 8AM
</commit_message>
<xml_diff>
--- a/WalletFundAddedStatement.xlsx
+++ b/WalletFundAddedStatement.xlsx
@@ -51,11 +51,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -87,16 +87,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -118,29 +124,39 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -156,7 +172,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -170,20 +186,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -192,40 +194,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -264,7 +264,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,7 +336,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -288,7 +384,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -300,91 +420,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,49 +438,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,6 +475,45 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -487,17 +526,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -520,38 +550,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -560,15 +560,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -578,130 +578,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -742,7 +742,7 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1067,9 +1067,9 @@
   <dimension ref="A1:I220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1122,31 +1122,31 @@
       </c>
       <c r="C2" s="7">
         <f>SUM(C3:C220)</f>
-        <v>4085074</v>
+        <v>4232900</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D3:D220)</f>
-        <v>3868820.14</v>
+        <v>4008821.03</v>
       </c>
       <c r="E2" s="8">
         <f>C2-D2</f>
-        <v>216253.859999999</v>
+        <v>224078.969999999</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F3:F220)</f>
-        <v>216253.86</v>
+        <v>224078.97</v>
       </c>
       <c r="G2" s="10">
         <f>C2-H2</f>
-        <v>61501.0543999998</v>
+        <v>63726.1287999996</v>
       </c>
       <c r="H2" s="7">
         <f>SUM(H3:H220)</f>
-        <v>4023572.9456</v>
+        <v>4169173.8712</v>
       </c>
       <c r="I2" s="10">
         <f>SUM(I3:I220)</f>
-        <v>61501.0543999999</v>
+        <v>63726.1287999999</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:9">
@@ -2172,22 +2172,37 @@
         <v>2066.88560000001</v>
       </c>
     </row>
-    <row r="34" spans="6:9">
-      <c r="F34" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="G34" s="11" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="H34" s="11" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I34" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+    <row r="34" spans="1:9">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2">
+        <v>26304590</v>
+      </c>
+      <c r="C34" s="11">
+        <v>147826</v>
+      </c>
+      <c r="D34" s="11">
+        <v>140000.89</v>
+      </c>
+      <c r="E34" s="12">
+        <v>44248</v>
+      </c>
+      <c r="F34" s="11">
+        <f t="shared" si="4"/>
+        <v>7825.10999999999</v>
+      </c>
+      <c r="G34" s="11">
+        <f t="shared" si="5"/>
+        <v>5.58932875355291</v>
+      </c>
+      <c r="H34" s="11">
+        <f t="shared" si="6"/>
+        <v>145600.9256</v>
+      </c>
+      <c r="I34" s="11">
+        <f t="shared" si="7"/>
+        <v>2225.07439999998</v>
       </c>
     </row>
     <row r="35" spans="6:9">

</xml_diff>